<commit_message>
Aurelija ir Gediminas baigia
</commit_message>
<xml_diff>
--- a/Dienynas JAVA 0522.xlsx
+++ b/Dienynas JAVA 0522.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19440" windowHeight="9555" tabRatio="793" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19440" windowHeight="9555" tabRatio="793" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1. Tarnyb. stotys" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="205">
   <si>
     <t>mėnuo / diena</t>
   </si>
@@ -573,6 +573,69 @@
   </si>
   <si>
     <t>09 30</t>
+  </si>
+  <si>
+    <t>10 01</t>
+  </si>
+  <si>
+    <t>10 02</t>
+  </si>
+  <si>
+    <t>10 03</t>
+  </si>
+  <si>
+    <t>10 04</t>
+  </si>
+  <si>
+    <t>10 07</t>
+  </si>
+  <si>
+    <t>10 10</t>
+  </si>
+  <si>
+    <t>10 08</t>
+  </si>
+  <si>
+    <t>10 09</t>
+  </si>
+  <si>
+    <t>10 11</t>
+  </si>
+  <si>
+    <t>10 14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>10 15</t>
+  </si>
+  <si>
+    <t>10 16</t>
+  </si>
+  <si>
+    <t>10 17</t>
+  </si>
+  <si>
+    <t>10 18</t>
+  </si>
+  <si>
+    <t>10 21</t>
+  </si>
+  <si>
+    <t>10 22</t>
+  </si>
+  <si>
+    <t>10 23</t>
+  </si>
+  <si>
+    <t>10 24</t>
+  </si>
+  <si>
+    <t>10 25</t>
+  </si>
+  <si>
+    <t>10 28</t>
   </si>
 </sst>
 </file>
@@ -867,6 +930,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -884,9 +950,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1279,10 +1342,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -1330,25 +1393,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="38" t="s">
+      <c r="AB3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AD3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="15" t="s">
         <v>63</v>
       </c>
@@ -1394,11 +1457,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
@@ -2015,7 +2078,7 @@
   <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,10 +2165,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -2120,13 +2183,27 @@
       <c r="F3" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>139</v>
+      </c>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
@@ -2141,25 +2218,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="38" t="s">
+      <c r="AB3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AD3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="14" t="s">
         <v>62</v>
       </c>
@@ -2172,13 +2249,27 @@
       <c r="F4" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+      <c r="G4" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>115</v>
+      </c>
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
@@ -2193,11 +2284,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
@@ -2218,13 +2309,27 @@
       <c r="F5" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="G5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>96</v>
+      </c>
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
       <c r="P5" s="18"/>
@@ -2320,7 +2425,9 @@
       <c r="X7" s="18"/>
       <c r="Y7" s="18"/>
       <c r="Z7" s="18"/>
-      <c r="AB7" s="18"/>
+      <c r="AB7" s="18" t="s">
+        <v>187</v>
+      </c>
       <c r="AC7" s="10">
         <v>8</v>
       </c>
@@ -2359,7 +2466,9 @@
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
       <c r="Z8" s="18"/>
-      <c r="AB8" s="18"/>
+      <c r="AB8" s="18" t="s">
+        <v>188</v>
+      </c>
       <c r="AC8" s="10">
         <v>8</v>
       </c>
@@ -2439,7 +2548,9 @@
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
       <c r="Z10" s="18"/>
-      <c r="AB10" s="18"/>
+      <c r="AB10" s="18" t="s">
+        <v>190</v>
+      </c>
       <c r="AC10" s="10">
         <v>8</v>
       </c>
@@ -2478,7 +2589,9 @@
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
       <c r="Z11" s="18"/>
-      <c r="AB11" s="18"/>
+      <c r="AB11" s="18" t="s">
+        <v>191</v>
+      </c>
       <c r="AC11" s="10">
         <v>8</v>
       </c>
@@ -2517,7 +2630,9 @@
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
       <c r="Z12" s="18"/>
-      <c r="AB12" s="18"/>
+      <c r="AB12" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="AC12" s="10">
         <v>8</v>
       </c>
@@ -2597,7 +2712,9 @@
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
       <c r="Z14" s="18"/>
-      <c r="AB14" s="18"/>
+      <c r="AB14" s="18" t="s">
+        <v>192</v>
+      </c>
       <c r="AC14" s="10">
         <v>8</v>
       </c>
@@ -2677,7 +2794,9 @@
       <c r="X16" s="18"/>
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
-      <c r="AB16" s="18"/>
+      <c r="AB16" s="18" t="s">
+        <v>193</v>
+      </c>
       <c r="AC16" s="10">
         <v>8</v>
       </c>
@@ -2833,10 +2952,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2888,25 +3007,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="34" t="s">
+      <c r="AB3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AD3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="15" t="s">
         <v>63</v>
       </c>
@@ -2956,11 +3075,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
     </row>
     <row r="5" spans="1:32" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -3580,8 +3699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3667,10 +3786,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="33" t="s">
@@ -3730,31 +3849,37 @@
       <c r="U3" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
+      <c r="V3" s="9">
+        <v>10</v>
+      </c>
+      <c r="W3" s="9">
+        <v>10</v>
+      </c>
+      <c r="X3" s="9">
+        <v>10</v>
+      </c>
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="34" t="s">
+      <c r="AB3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AD3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="9">
         <v>15</v>
       </c>
@@ -3812,17 +3937,23 @@
       <c r="U4" s="9">
         <v>30</v>
       </c>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
+      <c r="V4" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="W4" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="X4" s="33" t="s">
+        <v>94</v>
+      </c>
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
     </row>
     <row r="5" spans="1:32" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -3888,9 +4019,15 @@
       <c r="U5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
+      <c r="V5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
       <c r="AB5" s="10" t="s">
@@ -4477,7 +4614,9 @@
       <c r="Y19" s="10"/>
       <c r="Z19" s="10"/>
       <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
+      <c r="AB19" s="10" t="s">
+        <v>184</v>
+      </c>
       <c r="AC19" s="10">
         <v>8</v>
       </c>
@@ -4517,7 +4656,9 @@
       <c r="Y20" s="10"/>
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
-      <c r="AB20" s="10"/>
+      <c r="AB20" s="10" t="s">
+        <v>185</v>
+      </c>
       <c r="AC20" s="10">
         <v>8</v>
       </c>
@@ -4767,7 +4908,9 @@
       <c r="Y26" s="10"/>
       <c r="Z26" s="10"/>
       <c r="AA26" s="10"/>
-      <c r="AB26" s="10"/>
+      <c r="AB26" s="10" t="s">
+        <v>186</v>
+      </c>
       <c r="AC26" s="10">
         <v>8</v>
       </c>
@@ -4923,10 +5066,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="33" t="s">
@@ -4976,25 +5119,25 @@
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="34" t="s">
+      <c r="AB3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AD3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="33" t="s">
         <v>89</v>
       </c>
@@ -5042,11 +5185,11 @@
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
     </row>
     <row r="5" spans="1:32" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -5582,7 +5725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
@@ -5669,10 +5812,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -5693,13 +5836,13 @@
       <c r="H3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="34" t="s">
         <v>138</v>
       </c>
       <c r="L3" s="15" t="s">
@@ -5724,25 +5867,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="34" t="s">
+      <c r="AB3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AD3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="15" t="s">
         <v>114</v>
       </c>
@@ -5792,11 +5935,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -6375,7 +6518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB28" sqref="AB28"/>
     </sheetView>
   </sheetViews>
@@ -6462,10 +6605,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -6537,25 +6680,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="38" t="s">
+      <c r="AB3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AD3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="15" t="s">
         <v>136</v>
       </c>
@@ -6625,11 +6768,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -7679,8 +7822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7766,22 +7909,42 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>139</v>
+      </c>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
@@ -7797,35 +7960,55 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="34" t="s">
+      <c r="AB3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="34" t="s">
+      <c r="AD3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="34" t="s">
+      <c r="AE3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="34" t="s">
+      <c r="AF3" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>91</v>
+      </c>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
@@ -7841,11 +8024,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -7854,16 +8037,36 @@
       <c r="B5" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
@@ -7878,7 +8081,9 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="10"/>
+      <c r="AB5" s="10" t="s">
+        <v>195</v>
+      </c>
       <c r="AC5" s="10">
         <v>8</v>
       </c>
@@ -7915,7 +8120,9 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="10"/>
+      <c r="AB6" s="10" t="s">
+        <v>196</v>
+      </c>
       <c r="AC6" s="10">
         <v>8</v>
       </c>
@@ -7952,7 +8159,9 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="10"/>
+      <c r="AB7" s="10" t="s">
+        <v>197</v>
+      </c>
       <c r="AC7" s="10">
         <v>8</v>
       </c>
@@ -7989,7 +8198,9 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="10"/>
+      <c r="AB8" s="10" t="s">
+        <v>198</v>
+      </c>
       <c r="AC8" s="10">
         <v>8</v>
       </c>
@@ -8026,7 +8237,9 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="10"/>
+      <c r="AB9" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="AC9" s="10">
         <v>8</v>
       </c>
@@ -8063,7 +8276,9 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="10"/>
+      <c r="AB10" s="10" t="s">
+        <v>200</v>
+      </c>
       <c r="AC10" s="10">
         <v>8</v>
       </c>
@@ -8100,7 +8315,9 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AB11" s="10"/>
+      <c r="AB11" s="10" t="s">
+        <v>201</v>
+      </c>
       <c r="AC11" s="10">
         <v>8</v>
       </c>
@@ -8137,7 +8354,9 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="10"/>
+      <c r="AB12" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="AC12" s="10">
         <v>8</v>
       </c>
@@ -8174,7 +8393,9 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="10"/>
+      <c r="AB13" s="10" t="s">
+        <v>203</v>
+      </c>
       <c r="AC13" s="10">
         <v>8</v>
       </c>
@@ -8211,7 +8432,9 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="10"/>
+      <c r="AB14" s="10" t="s">
+        <v>204</v>
+      </c>
       <c r="AC14" s="10">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Aurelijos ir Gedimino zurnalai
</commit_message>
<xml_diff>
--- a/Dienynas JAVA 0522.xlsx
+++ b/Dienynas JAVA 0522.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="206">
   <si>
     <t>mėnuo / diena</t>
   </si>
@@ -636,6 +636,9 @@
   </si>
   <si>
     <t>10 28</t>
+  </si>
+  <si>
+    <t>10 29</t>
   </si>
 </sst>
 </file>
@@ -6461,7 +6464,7 @@
       </c>
       <c r="AF16" s="10"/>
     </row>
-    <row r="17" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -7823,7 +7826,7 @@
   <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7945,7 +7948,9 @@
       <c r="L3" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="M3" s="15"/>
+      <c r="M3" s="15" t="s">
+        <v>139</v>
+      </c>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
@@ -8009,7 +8014,9 @@
       <c r="L4" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="M4" s="15"/>
+      <c r="M4" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
@@ -8067,7 +8074,9 @@
       <c r="L5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
@@ -8444,7 +8453,7 @@
       <c r="AE14" s="10"/>
       <c r="AF14" s="10"/>
     </row>
-    <row r="15" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -8471,7 +8480,9 @@
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
-      <c r="AB15" s="10"/>
+      <c r="AB15" s="10" t="s">
+        <v>205</v>
+      </c>
       <c r="AC15" s="10">
         <v>4</v>
       </c>

</xml_diff>